<commit_message>
Added method that forces timely deliveries first, but might have been the wrong approach.
</commit_message>
<xml_diff>
--- a/WGUPS Distance Table.xlsx
+++ b/WGUPS Distance Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wessl\PycharmProjects\WGUPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D0BA62-BA3D-40B5-B3BC-4132B30DE061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59DE05E-99F5-4792-B635-E9134334B384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="9516" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -944,9 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM46" sqref="AM46"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3153,41 +3151,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Vendor xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">N/A</Vendor>
-    <Course_x0020_title xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <Launch_x0020_Date xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <Discipline xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <Course_x0020_short_x0020_name xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <SME xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <Course_x0020_code xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <qrac xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <Step_x0020_Completed xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
-      <Value>N/A</Value>
-    </Step_x0020_Completed>
-    <Course_x0020_number xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <d5fh xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <Publication_x0020_Date xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
-    <Assessment_x0020_Type xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
-      <Value>Objective</Value>
-    </Assessment_x0020_Type>
-    <Editor0 xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Editor0>
-    <Doc_x0020_Type xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
-    <Performance_x0020_Steps_x0020_Completed xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
-      <Value>N/A</Value>
-    </Performance_x0020_Steps_x0020_Completed>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A30F1838F1A9C4C8369A1109B92D3A0" ma:contentTypeVersion="25" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd847eb69213a28af7045ac4fae54026">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf660112-59e0-48e5-9b60-3f2262d4e05d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="20cce8b9bdf545eb805bf21ed5ebd307" ns2:_="">
     <xsd:import namespace="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
@@ -3523,6 +3486,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Vendor xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">N/A</Vendor>
+    <Course_x0020_title xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <Launch_x0020_Date xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <Discipline xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <Course_x0020_short_x0020_name xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <SME xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <Course_x0020_code xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <qrac xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <Step_x0020_Completed xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
+      <Value>N/A</Value>
+    </Step_x0020_Completed>
+    <Course_x0020_number xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <d5fh xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <Publication_x0020_Date xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d" xsi:nil="true"/>
+    <Assessment_x0020_Type xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
+      <Value>Objective</Value>
+    </Assessment_x0020_Type>
+    <Editor0 xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Editor0>
+    <Doc_x0020_Type xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
+    <Performance_x0020_Steps_x0020_Completed xmlns="cf660112-59e0-48e5-9b60-3f2262d4e05d">
+      <Value>N/A</Value>
+    </Performance_x0020_Steps_x0020_Completed>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3533,22 +3531,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3C0A13F-316D-473E-94B4-B9D9AB2AECAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3566,6 +3548,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC12B168-B9E1-4151-98F9-C97DA1AB8BBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cf660112-59e0-48e5-9b60-3f2262d4e05d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51ED99C8-D91C-4521-83EC-2A0A02D58674}">
   <ds:schemaRefs>

</xml_diff>